<commit_message>
xls cleaned + qst article added
</commit_message>
<xml_diff>
--- a/RF_Tap.xlsx
+++ b/RF_Tap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\RF_Tap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A086CF-E1AD-4AA4-AE45-423307EEC125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAC3E3A-BD41-4E5B-8F74-8377A65F27C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14D1D72B-EE71-4E4C-A43A-C8F3F42954EF}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
-  <si>
-    <t>In</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>R1A</t>
   </si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>GND</t>
-  </si>
-  <si>
-    <t>RF Tap Out</t>
   </si>
   <si>
     <t>R1</t>
@@ -260,15 +254,125 @@
   <si>
     <t>Pr2.2</t>
   </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RFTapOut</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In</t>
+    </r>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>Resistor power rating calculation</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>1/3P=</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <t>Uin (for 84,5W input power)=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -340,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +477,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77F4859-422B-4272-B810-4C51CBA49392}">
   <dimension ref="D4:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,56 +832,59 @@
     <col min="21" max="21" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="5:21" x14ac:dyDescent="0.25">
       <c r="I5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" s="7">
         <v>1E-3</v>
       </c>
       <c r="N5" s="8">
-        <f>M5*($F$17/($F$15+$F$17))</f>
+        <f>M5*($F$20/($F$18+$F$20))</f>
         <v>2.0310633213859019E-5</v>
       </c>
       <c r="O5" s="6">
@@ -803,15 +912,18 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="6" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N6" s="8">
-        <f>M6*($F$17/($F$15+$F$17))</f>
+        <f>M6*($F$20/($F$18+$F$20))</f>
         <v>1.015531660692951E-4</v>
       </c>
       <c r="O6" s="6">
@@ -839,15 +951,18 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="7" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" s="7">
         <v>0.01</v>
       </c>
       <c r="N7" s="8">
-        <f>M7*($F$17/($F$15+$F$17))</f>
+        <f>M7*($F$20/($F$18+$F$20))</f>
         <v>2.0310633213859019E-4</v>
       </c>
       <c r="O7" s="6">
@@ -875,15 +990,18 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="8" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="I8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" s="7">
         <v>0.05</v>
       </c>
       <c r="N8" s="8">
-        <f>M8*($F$17/($F$15+$F$17))</f>
+        <f>M8*($F$20/($F$18+$F$20))</f>
         <v>1.0155316606929509E-3</v>
       </c>
       <c r="O8" s="6">
@@ -911,15 +1029,18 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="9" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" s="7">
         <v>0.1</v>
       </c>
       <c r="N9" s="8">
-        <f>M9*($F$17/($F$15+$F$17))</f>
+        <f>M9*($F$20/($F$18+$F$20))</f>
         <v>2.0310633213859019E-3</v>
       </c>
       <c r="O9" s="6">
@@ -947,15 +1068,18 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="10" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M10" s="7">
         <v>0.5</v>
       </c>
       <c r="N10" s="8">
-        <f>M10*($F$17/($F$15+$F$17))</f>
+        <f>M10*($F$20/($F$18+$F$20))</f>
         <v>1.0155316606929509E-2</v>
       </c>
       <c r="O10" s="6">
@@ -983,15 +1107,12 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="11" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="M11" s="7">
         <v>1</v>
       </c>
       <c r="N11" s="8">
-        <f>M11*($F$17/($F$15+$F$17))</f>
+        <f>M11*($F$20/($F$18+$F$20))</f>
         <v>2.0310633213859019E-2</v>
       </c>
       <c r="O11" s="6">
@@ -1019,137 +1140,133 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="12" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="M12" s="7">
+        <v>5</v>
+      </c>
+      <c r="N12" s="8">
+        <f>M12*($F$20/($F$18+$F$20))</f>
+        <v>0.1015531660692951</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="0"/>
+        <v>-33.845530732299721</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="R12" s="11">
+        <f t="shared" si="2"/>
+        <v>26.989700043360187</v>
+      </c>
+      <c r="S12" s="9">
+        <f t="shared" si="3"/>
+        <v>2.0626091077395657E-4</v>
+      </c>
+      <c r="T12" s="11">
+        <f t="shared" si="2"/>
+        <v>-6.855830688939534</v>
+      </c>
+      <c r="U12" s="6">
+        <f t="shared" si="4"/>
+        <v>-33.845530732299721</v>
+      </c>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="7">
+        <v>10</v>
+      </c>
+      <c r="N13" s="8">
+        <f>M13*($F$20/($F$18+$F$20))</f>
+        <v>0.2031063321385902</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="0"/>
+        <v>-33.845530732299721</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R13" s="11">
+        <f t="shared" si="2"/>
+        <v>33.010299956639813</v>
+      </c>
+      <c r="S13" s="9">
+        <f t="shared" si="3"/>
+        <v>8.2504364309582629E-4</v>
+      </c>
+      <c r="T13" s="11">
+        <f t="shared" si="2"/>
+        <v>-0.83523077565991022</v>
+      </c>
+      <c r="U13" s="6">
+        <f t="shared" si="4"/>
+        <v>-33.845530732299721</v>
+      </c>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="7">
+        <v>15</v>
+      </c>
+      <c r="N14" s="8">
+        <f>M14*($F$20/($F$18+$F$20))</f>
+        <v>0.30465949820788529</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="0"/>
+        <v>-33.845530732299721</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="R14" s="11">
+        <f t="shared" si="2"/>
+        <v>36.532125137753432</v>
+      </c>
+      <c r="S14" s="9">
+        <f t="shared" si="3"/>
+        <v>1.8563481969656093E-3</v>
+      </c>
+      <c r="T14" s="11">
+        <f t="shared" si="2"/>
+        <v>2.6865944054537154</v>
+      </c>
+      <c r="U14" s="6">
+        <f t="shared" si="4"/>
+        <v>-33.845530732299721</v>
+      </c>
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
         <f>820</f>
         <v>820</v>
       </c>
-      <c r="M12" s="7">
-        <v>5</v>
-      </c>
-      <c r="N12" s="8">
-        <f>M12*($F$17/($F$15+$F$17))</f>
-        <v>0.1015531660692951</v>
-      </c>
-      <c r="O12" s="6">
-        <f t="shared" si="0"/>
-        <v>-33.845530732299721</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="R12" s="11">
-        <f t="shared" si="2"/>
-        <v>26.989700043360187</v>
-      </c>
-      <c r="S12" s="9">
-        <f t="shared" si="3"/>
-        <v>2.0626091077395657E-4</v>
-      </c>
-      <c r="T12" s="11">
-        <f t="shared" si="2"/>
-        <v>-6.855830688939534</v>
-      </c>
-      <c r="U12" s="6">
-        <f t="shared" si="4"/>
-        <v>-33.845530732299721</v>
-      </c>
-    </row>
-    <row r="13" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1">
-        <v>820</v>
-      </c>
-      <c r="M13" s="7">
-        <v>10</v>
-      </c>
-      <c r="N13" s="8">
-        <f>M13*($F$17/($F$15+$F$17))</f>
-        <v>0.2031063321385902</v>
-      </c>
-      <c r="O13" s="6">
-        <f t="shared" si="0"/>
-        <v>-33.845530732299721</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="R13" s="11">
-        <f t="shared" si="2"/>
-        <v>33.010299956639813</v>
-      </c>
-      <c r="S13" s="9">
-        <f t="shared" si="3"/>
-        <v>8.2504364309582629E-4</v>
-      </c>
-      <c r="T13" s="11">
-        <f t="shared" si="2"/>
-        <v>-0.83523077565991022</v>
-      </c>
-      <c r="U13" s="6">
-        <f t="shared" si="4"/>
-        <v>-33.845530732299721</v>
-      </c>
-    </row>
-    <row r="14" spans="5:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="4">
-        <v>820</v>
-      </c>
-      <c r="M14" s="7">
-        <v>15</v>
-      </c>
-      <c r="N14" s="8">
-        <f>M14*($F$17/($F$15+$F$17))</f>
-        <v>0.30465949820788529</v>
-      </c>
-      <c r="O14" s="6">
-        <f t="shared" si="0"/>
-        <v>-33.845530732299721</v>
-      </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
-      </c>
-      <c r="R14" s="11">
-        <f t="shared" si="2"/>
-        <v>36.532125137753432</v>
-      </c>
-      <c r="S14" s="9">
-        <f t="shared" si="3"/>
-        <v>1.8563481969656093E-3</v>
-      </c>
-      <c r="T14" s="11">
-        <f t="shared" si="2"/>
-        <v>2.6865944054537154</v>
-      </c>
-      <c r="U14" s="6">
-        <f t="shared" si="4"/>
-        <v>-33.845530732299721</v>
-      </c>
-    </row>
-    <row r="15" spans="5:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="5">
-        <f>SUM(F12:F14)</f>
-        <v>2460</v>
+      <c r="G15" s="1">
+        <v>817</v>
       </c>
       <c r="M15" s="7">
         <v>20</v>
       </c>
       <c r="N15" s="8">
-        <f>M15*($F$17/($F$15+$F$17))</f>
+        <f>M15*($F$20/($F$18+$F$20))</f>
         <v>0.40621266427718039</v>
       </c>
       <c r="O15" s="6">
@@ -1177,13 +1294,21 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="16" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="F16" s="1"/>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>820</v>
+      </c>
+      <c r="G16" s="1">
+        <v>817</v>
+      </c>
       <c r="M16" s="7">
         <v>25</v>
       </c>
       <c r="N16" s="8">
-        <f>M16*($F$17/($F$15+$F$17))</f>
+        <f>M16*($F$20/($F$18+$F$20))</f>
         <v>0.50776583034647549</v>
       </c>
       <c r="O16" s="6">
@@ -1211,18 +1336,21 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="17" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="5">
-        <v>51</v>
+    <row r="17" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>820</v>
+      </c>
+      <c r="G17" s="4">
+        <v>836</v>
       </c>
       <c r="M17" s="7">
         <v>30</v>
       </c>
       <c r="N17" s="8">
-        <f>M17*($F$17/($F$15+$F$17))</f>
+        <f>M17*($F$20/($F$18+$F$20))</f>
         <v>0.60931899641577059</v>
       </c>
       <c r="O17" s="6">
@@ -1250,12 +1378,23 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="18" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="5">
+        <f>SUM(F15:F17)</f>
+        <v>2460</v>
+      </c>
+      <c r="G18" s="5">
+        <f>SUM(G15:G17)</f>
+        <v>2470</v>
+      </c>
       <c r="M18" s="7">
         <v>35</v>
       </c>
       <c r="N18" s="8">
-        <f>M18*($F$17/($F$15+$F$17))</f>
+        <f>M18*($F$20/($F$18+$F$20))</f>
         <v>0.71087216248506568</v>
       </c>
       <c r="O18" s="6">
@@ -1284,11 +1423,12 @@
       </c>
     </row>
     <row r="19" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
       <c r="M19" s="7">
         <v>40</v>
       </c>
       <c r="N19" s="8">
-        <f>M19*($F$17/($F$15+$F$17))</f>
+        <f>M19*($F$20/($F$18+$F$20))</f>
         <v>0.81242532855436078</v>
       </c>
       <c r="O19" s="6">
@@ -1317,11 +1457,20 @@
       </c>
     </row>
     <row r="20" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5">
+        <v>51</v>
+      </c>
+      <c r="G20" s="5">
+        <v>51</v>
+      </c>
       <c r="M20" s="7">
         <v>45</v>
       </c>
       <c r="N20" s="8">
-        <f>M20*($F$17/($F$15+$F$17))</f>
+        <f>M20*($F$20/($F$18+$F$20))</f>
         <v>0.91397849462365588</v>
       </c>
       <c r="O20" s="6">
@@ -1350,14 +1499,11 @@
       </c>
     </row>
     <row r="21" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
       <c r="M21" s="7">
         <v>50</v>
       </c>
       <c r="N21" s="8">
-        <f>M21*($F$17/($F$15+$F$17))</f>
+        <f>M21*($F$20/($F$18+$F$20))</f>
         <v>1.015531660692951</v>
       </c>
       <c r="O21" s="6">
@@ -1386,14 +1532,11 @@
       </c>
     </row>
     <row r="22" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
       <c r="M22" s="7">
         <v>55</v>
       </c>
       <c r="N22" s="8">
-        <f>M22*($F$17/($F$15+$F$17))</f>
+        <f>M22*($F$20/($F$18+$F$20))</f>
         <v>1.117084826762246</v>
       </c>
       <c r="O22" s="6">
@@ -1426,7 +1569,7 @@
         <v>60</v>
       </c>
       <c r="N23" s="8">
-        <f>M23*($F$17/($F$15+$F$17))</f>
+        <f>M23*($F$20/($F$18+$F$20))</f>
         <v>1.2186379928315412</v>
       </c>
       <c r="O23" s="6">
@@ -1454,15 +1597,15 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="24" spans="5:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M24" s="7">
         <v>65</v>
       </c>
       <c r="N24" s="8">
-        <f>M24*($F$17/($F$15+$F$17))</f>
+        <f>M24*($F$20/($F$18+$F$20))</f>
         <v>1.3201911589008362</v>
       </c>
       <c r="O24" s="6">
@@ -1491,11 +1634,14 @@
       </c>
     </row>
     <row r="25" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
       <c r="M25" s="7">
         <v>70</v>
       </c>
       <c r="N25" s="8">
-        <f>M25*($F$17/($F$15+$F$17))</f>
+        <f>M25*($F$20/($F$18+$F$20))</f>
         <v>1.4217443249701314</v>
       </c>
       <c r="O25" s="6">
@@ -1528,7 +1674,7 @@
         <v>75</v>
       </c>
       <c r="N26" s="8">
-        <f>M26*($F$17/($F$15+$F$17))</f>
+        <f>M26*($F$20/($F$18+$F$20))</f>
         <v>1.5232974910394264</v>
       </c>
       <c r="O26" s="6">
@@ -1556,19 +1702,15 @@
         <v>-33.845530732299721</v>
       </c>
     </row>
-    <row r="27" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E27">
-        <f>F17/(F15+F17)</f>
-        <v>2.0310633213859019E-2</v>
-      </c>
-      <c r="F27">
-        <v>0.01</v>
+    <row r="27" spans="5:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>8</v>
       </c>
       <c r="M27" s="7">
         <v>80</v>
       </c>
       <c r="N27" s="8">
-        <f>M27*($F$17/($F$15+$F$17))</f>
+        <f>M27*($F$20/($F$18+$F$20))</f>
         <v>1.6248506571087216</v>
       </c>
       <c r="O27" s="6">
@@ -1601,7 +1743,7 @@
         <v>85</v>
       </c>
       <c r="N28" s="8">
-        <f>M28*($F$17/($F$15+$F$17))</f>
+        <f>M28*($F$20/($F$18+$F$20))</f>
         <v>1.7264038231780165</v>
       </c>
       <c r="O28" s="6">
@@ -1630,19 +1772,14 @@
       </c>
     </row>
     <row r="29" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E29">
-        <f>20*LOG(E27)</f>
-        <v>-33.845530732299721</v>
-      </c>
-      <c r="F29">
-        <f>20*LOG(F27)</f>
-        <v>-40</v>
+      <c r="E29" t="s">
+        <v>36</v>
       </c>
       <c r="M29" s="7">
         <v>90</v>
       </c>
       <c r="N29" s="8">
-        <f>M29*($F$17/($F$15+$F$17))</f>
+        <f>M29*($F$20/($F$18+$F$20))</f>
         <v>1.8279569892473118</v>
       </c>
       <c r="O29" s="6">
@@ -1675,7 +1812,7 @@
         <v>95</v>
       </c>
       <c r="N30" s="8">
-        <f>M30*($F$17/($F$15+$F$17))</f>
+        <f>M30*($F$20/($F$18+$F$20))</f>
         <v>1.9295101553166067</v>
       </c>
       <c r="O30" s="6">
@@ -1704,11 +1841,20 @@
       </c>
     </row>
     <row r="31" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31">
+        <v>65</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
       <c r="M31" s="7">
         <v>100</v>
       </c>
       <c r="N31" s="8">
-        <f>M31*($F$17/($F$15+$F$17))</f>
+        <f>M31*($F$20/($F$18+$F$20))</f>
         <v>2.031063321385902</v>
       </c>
       <c r="O31" s="6">
@@ -1738,46 +1884,67 @@
     </row>
     <row r="32" spans="5:23" x14ac:dyDescent="0.25">
       <c r="U32" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="V32" s="1">
         <v>50</v>
       </c>
       <c r="W32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <f>51*99</f>
-        <v>5049</v>
+      <c r="G33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="14">
+        <f>H31/(F18+F20)</f>
+        <v>2.5886101154918358E-2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F34">
-        <f>E33/820</f>
-        <v>6.1573170731707316</v>
+      <c r="G34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34">
+        <f>H33*H31*F18/(F18+F20)</f>
+        <v>1.648421973186557</v>
+      </c>
+      <c r="I34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" t="s">
+        <v>41</v>
+      </c>
+      <c r="K34" s="15">
+        <f>H34/3</f>
+        <v>0.54947399106218564</v>
+      </c>
+      <c r="L34" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F35">
-        <f>820*6</f>
-        <v>4920</v>
+      <c r="G35" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="13">
+        <f>H33*H31*F20/(F18+F20)</f>
+        <v>3.4174601883135945E-2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F36">
-        <f>E33-F35</f>
-        <v>129</v>
-      </c>
-      <c r="G36" s="12">
-        <f>F36/E33</f>
-        <v>2.5549613784907901E-2</v>
-      </c>
+      <c r="G36" s="12"/>
     </row>
     <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O41">
         <v>51</v>
@@ -1785,7 +1952,7 @@
     </row>
     <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="N42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O42">
         <v>5</v>
@@ -1793,7 +1960,7 @@
     </row>
     <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O43" s="13">
         <f>O42*2/O41</f>
@@ -1843,10 +2010,10 @@
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.25">
@@ -1859,12 +2026,12 @@
         <v>5040</v>
       </c>
       <c r="M50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H51">
         <v>70</v>
@@ -1872,7 +2039,7 @@
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H52">
         <f>H51/F50</f>
@@ -1881,7 +2048,7 @@
     </row>
     <row r="54" spans="4:15" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H54">
         <f>H52^2*650</f>
@@ -1896,7 +2063,7 @@
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H56">
         <f>H52^2*2200</f>

</xml_diff>